<commit_message>
update read connections and supermatrix example
</commit_message>
<xml_diff>
--- a/Examples/Dictionary/Input/ExpN_readSupermatrix.xlsx
+++ b/Examples/Dictionary/Input/ExpN_readSupermatrix.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shared/GITHUB/AhpAnpLib/Examples/Dictionary/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F445B52D-0055-E54B-B3C2-49E695981367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A70772-543F-F54F-9F57-CAF595260656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37580" yWindow="3140" windowWidth="23900" windowHeight="10380" xr2:uid="{85FBE8EF-A2A3-FF4A-A4E5-6C5A2BBF521C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16700" xr2:uid="{85FBE8EF-A2A3-FF4A-A4E5-6C5A2BBF521C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Supermatrix" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>

</xml_diff>